<commit_message>
written new code for read excel.
</commit_message>
<xml_diff>
--- a/SeleniumTest/src/excelExportAndFileIO/ExportExcel.xlsx
+++ b/SeleniumTest/src/excelExportAndFileIO/ExportExcel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14790" windowHeight="6345"/>
   </bookViews>
   <sheets>
     <sheet name="ExcelGuru99Demo" sheetId="1" r:id="rId1"/>
@@ -12,16 +12,65 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>mukesh</t>
   </si>
   <si>
     <t>priyanks</t>
+  </si>
+  <si>
+    <t>reegret</t>
+  </si>
+  <si>
+    <t>retert</t>
+  </si>
+  <si>
+    <t>weewrew</t>
+  </si>
+  <si>
+    <t>kjjhjkhkj</t>
+  </si>
+  <si>
+    <t>dfdfdsf</t>
+  </si>
+  <si>
+    <t>dfdsfdsf</t>
+  </si>
+  <si>
+    <t>rrtfdf</t>
+  </si>
+  <si>
+    <t>fddsfdf</t>
+  </si>
+  <si>
+    <t>fdsfsdf</t>
+  </si>
+  <si>
+    <t>dfdsf</t>
+  </si>
+  <si>
+    <t>dsfsf</t>
+  </si>
+  <si>
+    <t>rt4tew</t>
+  </si>
+  <si>
+    <t>tretertr</t>
+  </si>
+  <si>
+    <t>retretret</t>
+  </si>
+  <si>
+    <t>retertert</t>
+  </si>
+  <si>
+    <t>retret</t>
   </si>
 </sst>
 </file>
@@ -353,22 +402,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>